<commit_message>
Updated readme and neural_network_final_results
</commit_message>
<xml_diff>
--- a/neural_network_final_results.xlsx
+++ b/neural_network_final_results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8544" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8544"/>
   </bookViews>
   <sheets>
     <sheet name="Test Summary" sheetId="3" r:id="rId1"/>
@@ -2302,7 +2302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -22594,7 +22594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1048559" sqref="E1048559"/>
     </sheetView>
   </sheetViews>

</xml_diff>